<commit_message>
Added multiple recipe functionality
Added an extra filter column to filter on a list of recipes.
</commit_message>
<xml_diff>
--- a/Pao de qeijo.xlsx
+++ b/Pao de qeijo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lkrigun\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74EB8B80-D13F-4671-94F3-630679EBEF87}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EA01AD2-BCE0-4C7F-9679-21BAE94704DC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16790" yWindow="5150" windowWidth="18320" windowHeight="13880" xr2:uid="{5E09834D-B4A4-4C05-B6C1-D1F11C2846DF}"/>
+    <workbookView xWindow="5400" yWindow="4020" windowWidth="18320" windowHeight="13880" xr2:uid="{5E09834D-B4A4-4C05-B6C1-D1F11C2846DF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="30">
   <si>
     <t>weight</t>
   </si>
@@ -90,6 +90,39 @@
   </si>
   <si>
     <t>Total Weight g</t>
+  </si>
+  <si>
+    <t>recipe</t>
+  </si>
+  <si>
+    <t>pao de queijo</t>
+  </si>
+  <si>
+    <t>Farina</t>
+  </si>
+  <si>
+    <t>Acqua</t>
+  </si>
+  <si>
+    <t>Lievito di birra</t>
+  </si>
+  <si>
+    <t>Sale</t>
+  </si>
+  <si>
+    <t>quantity</t>
+  </si>
+  <si>
+    <t>Pizza Lievito di birra</t>
+  </si>
+  <si>
+    <t>Lievito naturale</t>
+  </si>
+  <si>
+    <t>Pizza Lievito naturale</t>
+  </si>
+  <si>
+    <t>notes</t>
   </si>
 </sst>
 </file>
@@ -126,7 +159,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -143,6 +176,12 @@
         <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -153,31 +192,72 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="3" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="4">
-    <cellStyle name="Bad" xfId="3" builtinId="27"/>
-    <cellStyle name="Good" xfId="2" builtinId="26"/>
+  <cellStyles count="3">
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Warning Text" xfId="1" builtinId="11"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="4">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF9C0006"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -198,20 +278,28 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DD426698-87A5-4505-B49C-8A65E9263A48}" name="Table1" displayName="Table1" ref="A1:E11" totalsRowCount="1">
-  <autoFilter ref="A1:E10" xr:uid="{75ADE708-D534-4AEE-8651-9278AB3EB6B0}"/>
-  <tableColumns count="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DD426698-87A5-4505-B49C-8A65E9263A48}" name="Table1" displayName="Table1" ref="A1:G21" totalsRowCount="1">
+  <autoFilter ref="A1:G20" xr:uid="{75ADE708-D534-4AEE-8651-9278AB3EB6B0}">
+    <filterColumn colId="5">
+      <filters>
+        <filter val="pao de queijo"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
+  <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{723BA3DE-3F88-4217-9887-CD5D8AF49A49}" name="Ingrediens" totalsRowLabel="Total"/>
-    <tableColumn id="2" xr3:uid="{3EA5B7BA-6D22-4BEB-B4F1-C2F4D5DC2295}" name="weight"/>
-    <tableColumn id="3" xr3:uid="{0AC49A8D-2DD6-4AC3-812F-B129733C0C7B}" name="Total Weight g" totalsRowFunction="sum" dataDxfId="1">
+    <tableColumn id="3" xr3:uid="{0AC49A8D-2DD6-4AC3-812F-B129733C0C7B}" name="Total Weight g" totalsRowFunction="sum" dataDxfId="3">
       <calculatedColumnFormula>Table1[[#This Row],[weight]]*Table1[[#Totals],[Coeficient]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{7DC4B8CC-02D0-4D8E-977C-C49A534F4053}" name="I have" totalsRowFunction="custom" dataCellStyle="Good" totalsRowCellStyle="Bad">
+    <tableColumn id="4" xr3:uid="{7DC4B8CC-02D0-4D8E-977C-C49A534F4053}" name="I have" totalsRowFunction="custom" totalsRowDxfId="1" dataCellStyle="Good">
       <totalsRowFormula>_xlfn.XLOOKUP(Table1[[#Totals],[Coeficient]],Table1[Coeficient],Table1[Ingrediens],"NA",0,1)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{8B78C24C-0833-46B2-98D6-8F0F0DB70DE3}" name="Coeficient" totalsRowFunction="min" dataDxfId="0" totalsRowCellStyle="Warning Text">
+    <tableColumn id="2" xr3:uid="{3EA5B7BA-6D22-4BEB-B4F1-C2F4D5DC2295}" name="weight" dataCellStyle="Good"/>
+    <tableColumn id="5" xr3:uid="{8B78C24C-0833-46B2-98D6-8F0F0DB70DE3}" name="Coeficient" totalsRowFunction="min" dataDxfId="2" totalsRowDxfId="0">
       <calculatedColumnFormula>Table1[[#This Row],[I have]]/Table1[[#This Row],[weight]]</calculatedColumnFormula>
     </tableColumn>
+    <tableColumn id="6" xr3:uid="{C854ECDD-9E69-4BFA-B0FF-16CD58250701}" name="recipe"/>
+    <tableColumn id="7" xr3:uid="{4885CA0B-5236-40AE-9EB9-D65090296851}" name="notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -514,242 +602,474 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9230FA1-7E54-4C12-AED1-FDB6F4295E2C}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="13.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="0" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="15.26953125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.6328125" customWidth="1"/>
-    <col min="5" max="5" width="11.1796875" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.1796875" customWidth="1"/>
+    <col min="6" max="6" width="17.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>15</v>
       </c>
       <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
         <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" t="s">
-        <v>13</v>
       </c>
       <c r="E1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2">
+        <f>Table1[[#This Row],[weight]]*Table1[[#Totals],[Coeficient]]</f>
         <v>320</v>
       </c>
-      <c r="C2">
-        <f>Table1[[#This Row],[weight]]*Table1[[#Totals],[Coeficient]]</f>
+      <c r="C2" s="1"/>
+      <c r="D2">
         <v>320</v>
       </c>
-      <c r="D2" s="2"/>
       <c r="E2" t="str">
         <f>IF(Table1[[#This Row],[I have]]/Table1[[#This Row],[weight]]=0,"",Table1[[#This Row],[I have]]/Table1[[#This Row],[weight]])</f>
         <v/>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3">
+        <f>Table1[[#This Row],[weight]]*Table1[[#Totals],[Coeficient]]</f>
         <v>8</v>
       </c>
-      <c r="C3">
-        <f>Table1[[#This Row],[weight]]*Table1[[#Totals],[Coeficient]]</f>
+      <c r="C3" s="1"/>
+      <c r="D3">
         <v>8</v>
       </c>
-      <c r="D3" s="2"/>
       <c r="E3" t="str">
         <f>IF(Table1[[#This Row],[I have]]/Table1[[#This Row],[weight]]=0,"",Table1[[#This Row],[I have]]/Table1[[#This Row],[weight]])</f>
         <v/>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4">
+        <f>Table1[[#This Row],[weight]]*Table1[[#Totals],[Coeficient]]</f>
         <v>4</v>
       </c>
-      <c r="C4">
-        <f>Table1[[#This Row],[weight]]*Table1[[#Totals],[Coeficient]]</f>
+      <c r="C4" s="1"/>
+      <c r="D4">
         <v>4</v>
       </c>
-      <c r="D4" s="2"/>
       <c r="E4" t="str">
         <f>IF(Table1[[#This Row],[I have]]/Table1[[#This Row],[weight]]=0,"",Table1[[#This Row],[I have]]/Table1[[#This Row],[weight]])</f>
         <v/>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5">
+        <f>Table1[[#This Row],[weight]]*Table1[[#Totals],[Coeficient]]</f>
         <v>160</v>
       </c>
-      <c r="C5">
-        <f>Table1[[#This Row],[weight]]*Table1[[#Totals],[Coeficient]]</f>
+      <c r="C5" s="1"/>
+      <c r="D5">
         <v>160</v>
       </c>
-      <c r="D5" s="2"/>
       <c r="E5" t="str">
         <f>IF(Table1[[#This Row],[I have]]/Table1[[#This Row],[weight]]=0,"",Table1[[#This Row],[I have]]/Table1[[#This Row],[weight]])</f>
         <v/>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6">
+        <f>Table1[[#This Row],[weight]]*Table1[[#Totals],[Coeficient]]</f>
         <v>30</v>
       </c>
-      <c r="C6">
-        <f>Table1[[#This Row],[weight]]*Table1[[#Totals],[Coeficient]]</f>
+      <c r="C6" s="1"/>
+      <c r="D6">
         <v>30</v>
       </c>
-      <c r="D6" s="2"/>
       <c r="E6" t="str">
         <f>IF(Table1[[#This Row],[I have]]/Table1[[#This Row],[weight]]=0,"",Table1[[#This Row],[I have]]/Table1[[#This Row],[weight]])</f>
         <v/>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="B7">
+        <f>Table1[[#This Row],[weight]]*Table1[[#Totals],[Coeficient]]</f>
         <v>2</v>
       </c>
-      <c r="C7">
-        <f>Table1[[#This Row],[weight]]*Table1[[#Totals],[Coeficient]]</f>
+      <c r="C7" s="1"/>
+      <c r="D7">
         <v>2</v>
       </c>
-      <c r="D7" s="2"/>
       <c r="E7" t="str">
         <f>IF(Table1[[#This Row],[I have]]/Table1[[#This Row],[weight]]=0,"",Table1[[#This Row],[I have]]/Table1[[#This Row],[weight]])</f>
         <v/>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>7</v>
       </c>
       <c r="B8">
+        <f>Table1[[#This Row],[weight]]*Table1[[#Totals],[Coeficient]]</f>
         <v>100</v>
       </c>
-      <c r="C8">
-        <f>Table1[[#This Row],[weight]]*Table1[[#Totals],[Coeficient]]</f>
+      <c r="C8" s="1"/>
+      <c r="D8">
         <v>100</v>
       </c>
-      <c r="D8" s="2"/>
       <c r="E8" t="str">
         <f>IF(Table1[[#This Row],[I have]]/Table1[[#This Row],[weight]]=0,"",Table1[[#This Row],[I have]]/Table1[[#This Row],[weight]])</f>
         <v/>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>8</v>
       </c>
       <c r="B9">
+        <f>Table1[[#This Row],[weight]]*Table1[[#Totals],[Coeficient]]</f>
         <v>160</v>
       </c>
-      <c r="C9">
-        <f>Table1[[#This Row],[weight]]*Table1[[#Totals],[Coeficient]]</f>
+      <c r="C9" s="1"/>
+      <c r="D9">
         <v>160</v>
       </c>
-      <c r="D9" s="2"/>
       <c r="E9" t="str">
         <f>IF(Table1[[#This Row],[I have]]/Table1[[#This Row],[weight]]=0,"",Table1[[#This Row],[I have]]/Table1[[#This Row],[weight]])</f>
         <v/>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>17</v>
       </c>
       <c r="B10">
+        <f>Table1[[#This Row],[weight]]*Table1[[#Totals],[Coeficient]]</f>
         <v>1</v>
       </c>
-      <c r="C10">
-        <f>Table1[[#This Row],[weight]]*Table1[[#Totals],[Coeficient]]</f>
+      <c r="C10" s="1">
         <v>1</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10">
         <v>1</v>
       </c>
       <c r="E10">
         <f>IF(Table1[[#This Row],[I have]]/Table1[[#This Row],[weight]]=0,"",Table1[[#This Row],[I have]]/Table1[[#This Row],[weight]])</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="6">
+        <f>Table1[[#This Row],[weight]]*Table1[[#Totals],[Coeficient]]</f>
+        <v>450</v>
+      </c>
+      <c r="C11" s="1"/>
+      <c r="D11">
+        <v>450</v>
+      </c>
+      <c r="E11" t="str">
+        <f>IF(Table1[[#This Row],[I have]]/Table1[[#This Row],[weight]]=0,"",Table1[[#This Row],[I have]]/Table1[[#This Row],[weight]])</f>
+        <v/>
+      </c>
+      <c r="F11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="6">
+        <f>Table1[[#This Row],[weight]]*Table1[[#Totals],[Coeficient]]</f>
+        <v>325</v>
+      </c>
+      <c r="C12" s="1"/>
+      <c r="D12">
+        <v>325</v>
+      </c>
+      <c r="E12" t="str">
+        <f>IF(Table1[[#This Row],[I have]]/Table1[[#This Row],[weight]]=0,"",Table1[[#This Row],[I have]]/Table1[[#This Row],[weight]])</f>
+        <v/>
+      </c>
+      <c r="F12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="6">
+        <f>Table1[[#This Row],[weight]]*Table1[[#Totals],[Coeficient]]</f>
+        <v>10</v>
+      </c>
+      <c r="C13" s="1"/>
+      <c r="D13">
+        <v>10</v>
+      </c>
+      <c r="E13" t="str">
+        <f>IF(Table1[[#This Row],[I have]]/Table1[[#This Row],[weight]]=0,"",Table1[[#This Row],[I have]]/Table1[[#This Row],[weight]])</f>
+        <v/>
+      </c>
+      <c r="F13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="6">
+        <f>Table1[[#This Row],[weight]]*Table1[[#Totals],[Coeficient]]</f>
+        <v>10</v>
+      </c>
+      <c r="C14" s="1"/>
+      <c r="D14">
+        <v>10</v>
+      </c>
+      <c r="E14" t="str">
+        <f>IF(Table1[[#This Row],[I have]]/Table1[[#This Row],[weight]]=0,"",Table1[[#This Row],[I have]]/Table1[[#This Row],[weight]])</f>
+        <v/>
+      </c>
+      <c r="F14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="6">
+        <f>Table1[[#This Row],[weight]]*Table1[[#Totals],[Coeficient]]</f>
+        <v>2</v>
+      </c>
+      <c r="C15" s="1"/>
+      <c r="D15">
+        <v>2</v>
+      </c>
+      <c r="E15" t="str">
+        <f>IF(Table1[[#This Row],[I have]]/Table1[[#This Row],[weight]]=0,"",Table1[[#This Row],[I have]]/Table1[[#This Row],[weight]])</f>
+        <v/>
+      </c>
+      <c r="F15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="6">
+        <f>Table1[[#This Row],[weight]]*Table1[[#Totals],[Coeficient]]</f>
+        <v>170</v>
+      </c>
+      <c r="C16" s="1"/>
+      <c r="D16">
+        <v>170</v>
+      </c>
+      <c r="E16" t="str">
+        <f>IF(Table1[[#This Row],[I have]]/Table1[[#This Row],[weight]]=0,"",Table1[[#This Row],[I have]]/Table1[[#This Row],[weight]])</f>
+        <v/>
+      </c>
+      <c r="F16" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" s="6">
+        <f>Table1[[#This Row],[weight]]*Table1[[#Totals],[Coeficient]]</f>
+        <v>110</v>
+      </c>
+      <c r="C17" s="1"/>
+      <c r="D17">
+        <v>110</v>
+      </c>
+      <c r="E17" t="str">
+        <f>IF(Table1[[#This Row],[I have]]/Table1[[#This Row],[weight]]=0,"",Table1[[#This Row],[I have]]/Table1[[#This Row],[weight]])</f>
+        <v/>
+      </c>
+      <c r="F17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" s="6">
+        <f>Table1[[#This Row],[weight]]*Table1[[#Totals],[Coeficient]]</f>
+        <v>15</v>
+      </c>
+      <c r="C18" s="1"/>
+      <c r="D18">
+        <v>15</v>
+      </c>
+      <c r="E18" t="str">
+        <f>IF(Table1[[#This Row],[I have]]/Table1[[#This Row],[weight]]=0,"",Table1[[#This Row],[I have]]/Table1[[#This Row],[weight]])</f>
+        <v/>
+      </c>
+      <c r="F18" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="6">
+        <f>Table1[[#This Row],[weight]]*Table1[[#Totals],[Coeficient]]</f>
+        <v>6</v>
+      </c>
+      <c r="C19" s="1"/>
+      <c r="D19">
+        <v>6</v>
+      </c>
+      <c r="E19" t="str">
+        <f>IF(Table1[[#This Row],[I have]]/Table1[[#This Row],[weight]]=0,"",Table1[[#This Row],[I have]]/Table1[[#This Row],[weight]])</f>
+        <v/>
+      </c>
+      <c r="F19" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="6">
+        <f>Table1[[#This Row],[weight]]*Table1[[#Totals],[Coeficient]]</f>
+        <v>1</v>
+      </c>
+      <c r="C20" s="1"/>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20" t="str">
+        <f>IF(Table1[[#This Row],[I have]]/Table1[[#This Row],[weight]]=0,"",Table1[[#This Row],[I have]]/Table1[[#This Row],[weight]])</f>
+        <v/>
+      </c>
+      <c r="F20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
         <v>9</v>
       </c>
-      <c r="C11">
+      <c r="B21">
         <f>SUBTOTAL(109,Table1[Total Weight g])</f>
         <v>785</v>
       </c>
-      <c r="D11" s="3" t="str">
+      <c r="C21" s="5" t="str">
         <f>_xlfn.XLOOKUP(Table1[[#Totals],[Coeficient]],Table1[Coeficient],Table1[Ingrediens],"NA",0,1)</f>
         <v>batch quantity</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E21" s="4">
         <f>SUBTOTAL(105,Table1[Coeficient])</f>
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" s="4" t="s">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A24" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16" s="5" t="s">
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A25" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A15:E15"/>
-    <mergeCell ref="A16:E16"/>
+    <mergeCell ref="A24:E24"/>
+    <mergeCell ref="A25:E25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>